<commit_message>
Drugs@FDA: `submissions.submission_property_type.id` should be removed since this is an internal primary key without a meaning
</commit_message>
<xml_diff>
--- a/static/fields/drugsfda_reference.xlsx
+++ b/static/fields/drugsfda_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5742CBBD-CF25-8946-9DE3-7C56CD301414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A303E5-08EF-2848-A634-3BCEAC832B22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Field Name</t>
   </si>
@@ -288,13 +288,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>The code indicating the submission property type.</t>
-  </si>
-  <si>
-    <t>The id of the submission property type.</t>
   </si>
   <si>
     <t>The fields indicating the property type of the submission.</t>
@@ -1171,10 +1165,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,32 +1596,32 @@
         <v>58</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="C32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>62</v>
@@ -1641,7 +1635,7 @@
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>64</v>
@@ -1655,21 +1649,21 @@
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>66</v>
@@ -1748,7 +1742,7 @@
         <v>49</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1762,21 +1756,21 @@
         <v>3</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1784,13 +1778,13 @@
         <v>58</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1798,13 +1792,13 @@
         <v>58</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1812,26 +1806,12 @@
         <v>58</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="5" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drugs@FDA: `submissions.submission_property_type.id` should be removed since this is an internal primary key without a meaning (#207)
</commit_message>
<xml_diff>
--- a/static/fields/drugsfda_reference.xlsx
+++ b/static/fields/drugsfda_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5742CBBD-CF25-8946-9DE3-7C56CD301414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A303E5-08EF-2848-A634-3BCEAC832B22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Field Name</t>
   </si>
@@ -288,13 +288,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>The code indicating the submission property type.</t>
-  </si>
-  <si>
-    <t>The id of the submission property type.</t>
   </si>
   <si>
     <t>The fields indicating the property type of the submission.</t>
@@ -1171,10 +1165,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,32 +1596,32 @@
         <v>58</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="C32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>62</v>
@@ -1641,7 +1635,7 @@
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>64</v>
@@ -1655,21 +1649,21 @@
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>66</v>
@@ -1748,7 +1742,7 @@
         <v>49</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1762,21 +1756,21 @@
         <v>3</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1784,13 +1778,13 @@
         <v>58</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1798,13 +1792,13 @@
         <v>58</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1812,26 +1806,12 @@
         <v>58</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="5" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>